<commit_message>
Update Excel sample file with correct database skills
- Use Electric, HVAC, Plumbing from database
- Use heating from database
- All skills now match the database exactly
- Ready to upload without skill errors
</commit_message>
<xml_diff>
--- a/bulk_upload_sample.xlsx
+++ b/bulk_upload_sample.xlsx
@@ -573,7 +573,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>electrical,hvac,plumbing</t>
+          <t>Electric,HVAC,Plumbing</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>electrical,hvac</t>
+          <t>Electric,HVAC</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>plumbing,heating</t>
+          <t>Plumbing,heating</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>electrical,hvac,plumbing</t>
+          <t>Electric,HVAC,Plumbing</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>electrical,hvac</t>
+          <t>Electric,HVAC</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>plumbing,heating</t>
+          <t>Plumbing,heating</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">

</xml_diff>

<commit_message>
Change ServiceRequest to single skill: One skill per service request
- Change required_skills (ManyToMany) to required_skill (ForeignKey)
- Update bulk upload service to use single skill
- Update admin to show single skill field
- Only technicians keep multiple skills (ManyToMany)
- Service requests now have exactly one required skill
- Create migration for database schema change
</commit_message>
<xml_diff>
--- a/bulk_upload_sample.xlsx
+++ b/bulk_upload_sample.xlsx
@@ -573,7 +573,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Electric,HVAC,Plumbing</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Gas Leak Repair</t>
+          <t>Electrical Repair</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Electric,HVAC</t>
+          <t>HVAC</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Electrical Fault</t>
+          <t>HVAC Maintenance</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Plumbing,heating</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Electric,HVAC,Plumbing</t>
+          <t>Electric</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Electric,HVAC</t>
+          <t>HVAC</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Plumbing,heating</t>
+          <t>Plumbing</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">

</xml_diff>